<commit_message>
charge subject place commentを作成
</commit_message>
<xml_diff>
--- a/draft.xlsx
+++ b/draft.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\マイドライブ\20240501\studyroom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{289B8490-58DF-498D-B28B-C1DB9B49CF9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4BAB20F-464E-42BD-AFE4-877798938E02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11295" firstSheet="1" activeTab="3" xr2:uid="{EC313A2C-D88C-4268-B62A-D14DFB7CC92B}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21615" windowHeight="11295" activeTab="1" xr2:uid="{EC313A2C-D88C-4268-B62A-D14DFB7CC92B}"/>
   </bookViews>
   <sheets>
     <sheet name="基本情報" sheetId="5" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="114">
   <si>
     <t>id</t>
     <phoneticPr fontId="1"/>
@@ -435,10 +435,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>!set</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>onopod !set 簿記2級</t>
     <rPh sb="12" eb="14">
       <t>ボキ</t>
@@ -642,10 +638,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>!moveto</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>onopod !moveto A12</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -742,6 +734,18 @@
   </si>
   <si>
     <t>→</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>!subject</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>!place</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>comment</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1189,198 +1193,222 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB01D54D-2177-4EDE-B257-0E709723DC25}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomRight" activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="15.375" customWidth="1"/>
-    <col min="2" max="2" width="18.625" customWidth="1"/>
-    <col min="3" max="3" width="36.75" customWidth="1"/>
-    <col min="4" max="4" width="69.125" customWidth="1"/>
-    <col min="5" max="5" width="67.625" customWidth="1"/>
+    <col min="2" max="2" width="15.375" customWidth="1"/>
+    <col min="3" max="3" width="18.625" customWidth="1"/>
+    <col min="4" max="4" width="36.75" customWidth="1"/>
+    <col min="5" max="5" width="69.125" customWidth="1"/>
+    <col min="6" max="6" width="67.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A1" s="4"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="E2" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="B1" s="4"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="F2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G2" t="s">
         <v>75</v>
       </c>
-      <c r="F2" t="s">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="B3" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
+      <c r="C3" t="s">
         <v>77</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="37.5" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" t="s">
+        <v>68</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D6" t="s">
+        <v>86</v>
+      </c>
+      <c r="E6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
+        <v>99</v>
+      </c>
+      <c r="B7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
+        <v>99</v>
+      </c>
+      <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="B9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="37.5" x14ac:dyDescent="0.4">
+      <c r="B10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" t="s">
         <v>78</v>
       </c>
-      <c r="C3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E3" t="s">
-        <v>73</v>
-      </c>
-      <c r="F3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="37.5" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D4" t="s">
-        <v>69</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="F4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A5" t="s">
-        <v>66</v>
-      </c>
-      <c r="B5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C5" t="s">
-        <v>68</v>
-      </c>
-      <c r="D5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A6" t="s">
-        <v>89</v>
-      </c>
-      <c r="B6" t="s">
-        <v>90</v>
-      </c>
-      <c r="C6" t="s">
-        <v>87</v>
-      </c>
-      <c r="D6" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C7" t="s">
-        <v>43</v>
-      </c>
-      <c r="D7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" t="s">
-        <v>40</v>
-      </c>
-      <c r="D8" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" t="s">
-        <v>50</v>
-      </c>
-      <c r="C9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="37.5" x14ac:dyDescent="0.4">
-      <c r="A10" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10" t="s">
-        <v>51</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="E10" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
+        <v>99</v>
+      </c>
+      <c r="B11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
+        <v>110</v>
+      </c>
+      <c r="B12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" t="s">
         <v>79</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A11" t="s">
-        <v>44</v>
-      </c>
-      <c r="B11" t="s">
-        <v>52</v>
-      </c>
-      <c r="C11" t="s">
-        <v>48</v>
-      </c>
-      <c r="D11" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A12" t="s">
-        <v>46</v>
-      </c>
-      <c r="B12" t="s">
-        <v>47</v>
-      </c>
-      <c r="C12" t="s">
-        <v>45</v>
-      </c>
-      <c r="D12" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
+        <v>110</v>
+      </c>
+      <c r="B13" t="s">
         <v>56</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>57</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>58</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1392,10 +1420,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06431C40-7286-4F6D-9456-C11ECEDB1A0F}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -1434,70 +1462,70 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
+        <v>113</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>29</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A9" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" t="s">
-        <v>25</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C12" t="s">
         <v>24</v>
@@ -1505,62 +1533,62 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>93</v>
+        <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>92</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B14" t="s">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B15" t="s">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B16" t="s">
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="B17" t="s">
-        <v>64</v>
+        <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>65</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B18" t="s">
         <v>64</v>
@@ -1571,12 +1599,23 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
+        <v>109</v>
+      </c>
+      <c r="B19" t="s">
+        <v>64</v>
+      </c>
+      <c r="C19" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A20" t="s">
         <v>8</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>29</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C20" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1590,7 +1629,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE3FB08B-0070-431A-8B01-AE62C0023292}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -1604,12 +1643,12 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B2" t="s">
         <v>13</v>
@@ -1626,7 +1665,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
@@ -1643,7 +1682,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B4" t="s">
         <v>17</v>
@@ -1660,7 +1699,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
@@ -1674,7 +1713,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
@@ -1683,12 +1722,12 @@
         <v>27</v>
       </c>
       <c r="E6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B7" t="s">
         <v>21</v>
@@ -1702,7 +1741,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.4">
@@ -1721,13 +1760,13 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E11" t="s">
         <v>10</v>
@@ -1735,13 +1774,13 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E12" t="s">
         <v>22</v>
@@ -1749,44 +1788,44 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B14" t="s">
         <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B15" t="s">
         <v>12</v>
       </c>
       <c r="C15" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D15" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>18</v>
@@ -1794,33 +1833,33 @@
     </row>
     <row r="16" spans="1:5" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B16" t="s">
         <v>12</v>
       </c>
       <c r="C16" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B17" t="s">
         <v>17</v>
       </c>
       <c r="C17" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E17" t="s">
         <v>19</v>
@@ -1828,13 +1867,13 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B18" t="s">
         <v>21</v>
       </c>
       <c r="C18" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E18" t="s">
         <v>20</v>

</xml_diff>